<commit_message>
fix(FN-3460): add two rows previously causing FP errors in facility utilisation cells
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FC436-0FE6-4DC5-9478-BF4C7E178814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Total fees accrued for the period</t>
+  </si>
+  <si>
+    <t>Crumpet GEF</t>
+  </si>
+  <si>
+    <t>Scone GEF</t>
+  </si>
+  <si>
+    <t>Crumpet exporter</t>
+  </si>
+  <si>
+    <t>Scone exporter</t>
   </si>
 </sst>
 </file>
@@ -202,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -348,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,26 +512,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +599,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,30 +667,82 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6">
+        <v>7000000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3938753.8</v>
+      </c>
+      <c r="G5" s="7">
+        <v>777</v>
+      </c>
+      <c r="H5" s="7">
+        <v>456</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <v>770000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>761579.37</v>
+      </c>
+      <c r="G6" s="7">
+        <v>777</v>
+      </c>
+      <c r="H6" s="7">
+        <v>456.77</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -691,7 +755,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -704,7 +768,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -717,14 +781,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -736,7 +800,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -749,7 +813,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -762,7 +826,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -771,7 +835,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -781,7 +845,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>

</xml_diff>

<commit_message>
fix(FN-3460): fix numerical rounding errors during report upload (#3546)
Co-authored-by: Christian McCaffery <cmccaffery@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FC436-0FE6-4DC5-9478-BF4C7E178814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Total fees accrued for the period</t>
+  </si>
+  <si>
+    <t>Crumpet GEF</t>
+  </si>
+  <si>
+    <t>Scone GEF</t>
+  </si>
+  <si>
+    <t>Crumpet exporter</t>
+  </si>
+  <si>
+    <t>Scone exporter</t>
   </si>
 </sst>
 </file>
@@ -202,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -348,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,26 +512,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +599,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,30 +667,82 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6">
+        <v>7000000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3938753.8</v>
+      </c>
+      <c r="G5" s="7">
+        <v>777</v>
+      </c>
+      <c r="H5" s="7">
+        <v>456</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <v>770000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>761579.37</v>
+      </c>
+      <c r="G6" s="7">
+        <v>777</v>
+      </c>
+      <c r="H6" s="7">
+        <v>456.77</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -691,7 +755,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -704,7 +768,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -717,14 +781,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -736,7 +800,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -749,7 +813,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -762,7 +826,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -771,7 +835,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -781,7 +845,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>

</xml_diff>

<commit_message>
fix(FN-3481): cherry-pick numerical rounding error fix from #3546 (targeting main) (#3565)
Co-authored-by: Christian McCaffery <cmccaffery@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FC436-0FE6-4DC5-9478-BF4C7E178814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Total fees accrued for the period</t>
+  </si>
+  <si>
+    <t>Crumpet GEF</t>
+  </si>
+  <si>
+    <t>Scone GEF</t>
+  </si>
+  <si>
+    <t>Crumpet exporter</t>
+  </si>
+  <si>
+    <t>Scone exporter</t>
   </si>
 </sst>
 </file>
@@ -202,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -348,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,26 +512,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +599,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,30 +667,82 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6">
+        <v>7000000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3938753.8</v>
+      </c>
+      <c r="G5" s="7">
+        <v>777</v>
+      </c>
+      <c r="H5" s="7">
+        <v>456</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <v>770000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>761579.37</v>
+      </c>
+      <c r="G6" s="7">
+        <v>777</v>
+      </c>
+      <c r="H6" s="7">
+        <v>456.77</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -691,7 +755,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -704,7 +768,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -717,14 +781,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -736,7 +800,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -749,7 +813,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -762,7 +826,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -771,7 +835,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -781,7 +845,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>

</xml_diff>

<commit_message>
fix(FN-3481): cherry-pick numerical rounding error fix from #3546 (targeting release-2.3) (#3564)
Co-authored-by: Christian McCaffery <cmccaffery@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FC436-0FE6-4DC5-9478-BF4C7E178814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Total fees accrued for the period</t>
+  </si>
+  <si>
+    <t>Crumpet GEF</t>
+  </si>
+  <si>
+    <t>Scone GEF</t>
+  </si>
+  <si>
+    <t>Crumpet exporter</t>
+  </si>
+  <si>
+    <t>Scone exporter</t>
   </si>
 </sst>
 </file>
@@ -202,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -348,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,26 +512,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +599,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,30 +667,82 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6">
+        <v>7000000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3938753.8</v>
+      </c>
+      <c r="G5" s="7">
+        <v>777</v>
+      </c>
+      <c r="H5" s="7">
+        <v>456</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20001371</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <v>770000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>761579.37</v>
+      </c>
+      <c r="G6" s="7">
+        <v>777</v>
+      </c>
+      <c r="H6" s="7">
+        <v>456.77</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -691,7 +755,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -704,7 +768,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -717,14 +781,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -736,7 +800,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -749,7 +813,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -762,7 +826,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -771,7 +835,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -781,7 +845,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>

</xml_diff>

<commit_message>
chore(FN-3225): code improvements and changes
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07940BE-7357-4B1B-8121-27931EAE5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>600000</v>
       </c>
       <c r="F2" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G2" s="7">
         <v>123</v>
@@ -616,7 +616,7 @@
         <v>600000</v>
       </c>
       <c r="F3" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G3" s="7">
         <v>150</v>
@@ -649,7 +649,7 @@
         <v>600000</v>
       </c>
       <c r="F4" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G4" s="7">
         <v>45</v>
@@ -684,7 +684,7 @@
         <v>7000000</v>
       </c>
       <c r="F5" s="7">
-        <v>3938753.8</v>
+        <v>761579.37</v>
       </c>
       <c r="G5" s="7">
         <v>777</v>

</xml_diff>

<commit_message>
feat(FN-3225): added validation for matching facility id currency and utilisation (#3513)
Co-authored-by: Zain Kassam <zkassam@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1591D52D-7C70-406B-B580-4E1FDD89423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07940BE-7357-4B1B-8121-27931EAE5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>600000</v>
       </c>
       <c r="F2" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G2" s="7">
         <v>123</v>
@@ -616,7 +616,7 @@
         <v>600000</v>
       </c>
       <c r="F3" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G3" s="7">
         <v>150</v>
@@ -649,7 +649,7 @@
         <v>600000</v>
       </c>
       <c r="F4" s="7">
-        <v>100000</v>
+        <v>761579.37</v>
       </c>
       <c r="G4" s="7">
         <v>45</v>
@@ -684,7 +684,7 @@
         <v>7000000</v>
       </c>
       <c r="F5" s="7">
-        <v>3938753.8</v>
+        <v>761579.37</v>
       </c>
       <c r="G5" s="7">
         <v>777</v>

</xml_diff>

<commit_message>
fix(FN-3460): fix invalid facility utilisation values -- all need to match as same facility id for all rows
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07940BE-7357-4B1B-8121-27931EAE5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4398BA-8278-4AB5-B2B1-8358544C14EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E5" sqref="E5:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,8 +522,7 @@
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="5" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="14.109375" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
@@ -681,13 +680,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="6">
-        <v>7000000</v>
+        <v>600000</v>
       </c>
       <c r="F5" s="7">
         <v>761579.37</v>
       </c>
       <c r="G5" s="7">
-        <v>777</v>
+        <v>3938753.8</v>
       </c>
       <c r="H5" s="7">
         <v>456</v>
@@ -713,13 +712,13 @@
         <v>7</v>
       </c>
       <c r="E6" s="6">
-        <v>770000</v>
+        <v>600000</v>
       </c>
       <c r="F6" s="7">
         <v>761579.37</v>
       </c>
       <c r="G6" s="7">
-        <v>777</v>
+        <v>761579.37</v>
       </c>
       <c r="H6" s="7">
         <v>456.77</v>

</xml_diff>

<commit_message>
fix(FN-3460): make all files match
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4398BA-8278-4AB5-B2B1-8358544C14EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F047A9-C5B8-48BC-B0A6-E91647AB83D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:H6"/>
+      <selection activeCell="E2" sqref="E2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,8 +522,7 @@
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="5" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="20.109375" customWidth="1"/>
@@ -579,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F2" s="7">
         <v>761579.37</v>
@@ -612,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F3" s="7">
         <v>761579.37</v>
@@ -645,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F4" s="7">
         <v>761579.37</v>
@@ -680,16 +679,16 @@
         <v>7</v>
       </c>
       <c r="E5" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F5" s="7">
         <v>761579.37</v>
       </c>
       <c r="G5" s="7">
+        <v>456</v>
+      </c>
+      <c r="H5" s="7">
         <v>3938753.8</v>
-      </c>
-      <c r="H5" s="7">
-        <v>456</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>7</v>
@@ -712,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F6" s="7">
         <v>761579.37</v>

</xml_diff>

<commit_message>
fix(FN-3460): fix invalid facility utilisation values in e2e report fixtures (#3584)
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWilliams\Downloads\git\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07940BE-7357-4B1B-8121-27931EAE5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F047A9-C5B8-48BC-B0A6-E91647AB83D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,9 +522,7 @@
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="5" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="11" width="20.109375" customWidth="1"/>
@@ -580,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F2" s="7">
         <v>761579.37</v>
@@ -613,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F3" s="7">
         <v>761579.37</v>
@@ -646,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="6">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="F4" s="7">
         <v>761579.37</v>
@@ -681,16 +679,16 @@
         <v>7</v>
       </c>
       <c r="E5" s="6">
-        <v>7000000</v>
+        <v>800000</v>
       </c>
       <c r="F5" s="7">
         <v>761579.37</v>
       </c>
       <c r="G5" s="7">
-        <v>777</v>
+        <v>456</v>
       </c>
       <c r="H5" s="7">
-        <v>456</v>
+        <v>3938753.8</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>7</v>
@@ -713,13 +711,13 @@
         <v>7</v>
       </c>
       <c r="E6" s="6">
-        <v>770000</v>
+        <v>800000</v>
       </c>
       <c r="F6" s="7">
         <v>761579.37</v>
       </c>
       <c r="G6" s="7">
-        <v>777</v>
+        <v>761579.37</v>
       </c>
       <c r="H6" s="7">
         <v>456.77</v>

</xml_diff>